<commit_message>
update codebook base file
</commit_message>
<xml_diff>
--- a/data/codebook_base_file.xlsx
+++ b/data/codebook_base_file.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lisch\3D Objects\prefer\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{583E639B-9402-4269-9D3F-9DD1FA0005E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44FB01AC-6256-4CEE-ACC2-35E0E8A616F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -933,7 +933,7 @@
     <t>"Married" here means both marriage and registered partnership. "Unmarried" couple means a couple who are not in marriage and not in registered partnership but CBS inferred that they are partners. This slightly overestimates the number of unmarried couples. Co-habiting with a partner (in an unmarried/unregistered union) is likely more accurately captured in HuisGenotenNetwerkTab based on tax information (e.g. being benefit partners)</t>
   </si>
   <si>
-    <t>Dutch education system includes several different tracks (mbo/vmbo - vocational education, havo - leads to applied higher education (applied higher educational institutions), vwo - leads to academic/theoretical higher education (universities)). Selection into tracks start after primary school. This classification reflects not only educational level but also tracks (e.g. practical bachelor programs (hbo) are distinguished from theoretical/academic (vwo)). For details about these different educational levels and meaning of each code see Standard Onderwijsindeling 2021 (https://www.cbs.nl/nl-nl/onze-diensten/methoden/classificaties/onderwijs-en-beroepen/standaard-onderwijsindeling--soi--/standaard-onderwijsindeling-2021)</t>
+    <t>Dutch education system includes several different tracks (mbo/vmbo - vocational education, havo - leads to applied higher education (applied higher educational institutions), vwo - leads to academic/theoretical higher education (universities)). Selection into tracks start after primary school. This classification reflects not only educational level but also tracks (e.g. practical bachelor programs (hbo) are distinguished from theoretical/academic (vwo)). For details about these different educational levels and meaning of each code see Standard Onderwijsindeling 2021 (https://www.cbs.nl/nl-nl/onze-diensten/methoden/classificaties/onderwijs-en-beroepen/standaard-onderwijsindeling--soi--/standaard-onderwijsindeling-2021). Brief description of SOI 2021 classification see here https://www.cbs.nl/nl-nl/onze-diensten/methoden/begrippen/onderwijsniveau-soi-2021</t>
   </si>
 </sst>
 </file>
@@ -1749,8 +1749,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F137"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C21" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+    <sheetView tabSelected="1" topLeftCell="D21" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>